<commit_message>
update flow voucher course information
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/voucher.xlsx
+++ b/src/main/resources/input_excel_file/booking/voucher.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" firstSheet="2" activeTab="6"/>
+    <workbookView windowWidth="28800" windowHeight="12180" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Booking_Voucher_Check" sheetId="1" r:id="rId1"/>
@@ -5240,8 +5240,8 @@
   <sheetPr/>
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
@@ -6560,8 +6560,8 @@
   <sheetPr/>
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>

</xml_diff>